<commit_message>
Made some minor changes
</commit_message>
<xml_diff>
--- a/Documents/comp3111 gantt chart.xlsx
+++ b/Documents/comp3111 gantt chart.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imc4kmacpro/Documents/COMP3111/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Tang\Documents\Academic_UN\Y3 Fall\COMP 3111\COMP 3111 Project\COMP 3111 Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39E0F9E-E386-483A-9DEE-ECD2BAC03301}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="458" windowWidth="28800" windowHeight="17543" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -68,7 +74,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -109,7 +115,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -117,14 +123,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-TW"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -142,10 +151,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.256466646434165"/>
-          <c:y val="0.13757686558383"/>
-          <c:w val="0.62167022644178"/>
-          <c:h val="0.811687854184553"/>
+          <c:x val="0.32276184737638069"/>
+          <c:y val="0.11326394944477892"/>
+          <c:w val="0.62167022644178005"/>
+          <c:h val="0.81168785418455303"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -210,35 +219,40 @@
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$9</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>43385.0</c:v>
+                  <c:v>43385</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43390.0</c:v>
+                  <c:v>43390</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43391.0</c:v>
+                  <c:v>43391</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43392.0</c:v>
+                  <c:v>43392</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43404.0</c:v>
+                  <c:v>43404</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43411.0</c:v>
+                  <c:v>43411</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43407.0</c:v>
+                  <c:v>43407</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43433.0</c:v>
+                  <c:v>43433</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2050-4009-951E-402C73C6881A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -305,32 +319,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2050-4009-951E-402C73C6881A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -400,8 +419,8 @@
         <c:axId val="-556778960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="43440.0"/>
-          <c:min val="43380.0"/>
+          <c:max val="43440"/>
+          <c:min val="43380"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -453,7 +472,7 @@
         <c:crossAx val="-558324736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="7.0"/>
+        <c:majorUnit val="7"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1062,7 +1081,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1342,19 +1367,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="177" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="39.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1368,7 +1391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1383,7 +1406,7 @@
         <v>43391</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1397,7 +1420,7 @@
         <v>43391</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1411,7 +1434,7 @@
         <v>43392</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1425,7 +1448,7 @@
         <v>43404</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1439,7 +1462,7 @@
         <v>43411</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1453,7 +1476,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1467,7 +1490,7 @@
         <v>43420</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>